<commit_message>
One image added to the before and after file, images added to one location.
</commit_message>
<xml_diff>
--- a/data/BeforeAndAfter.xlsx
+++ b/data/BeforeAndAfter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\landscapingUOB-api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3AE12F-5B21-470E-BE64-69E56FA07573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B3C698A-A362-456B-81C4-7DD161A8A99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="152">
   <si>
     <t>Location Type</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>https://i.postimg.cc/TP8M0zvP/DSC-0120.jpg</t>
-  </si>
-  <si>
-    <t>https://i.postimg.cc/GmdMt4q8/10-94.jpg</t>
   </si>
   <si>
     <t>S4</t>
@@ -527,6 +524,9 @@
   <si>
     <t>This slider presents a before-and-after comparison of the outdoor area at the Department of Architecture &amp; Interior Design. The project involved a complete redesign of the space, introducing natural grass and ornamental trees to enhance the visual quality of the area.
 The newly landscaped area has become more attractive and visually pleasing, creating a comfortable and inviting outdoor environment for visitors and users.</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/qM0Y3Pjj/DSC-0133.jpg</t>
   </si>
 </sst>
 </file>
@@ -594,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -610,12 +610,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -680,25 +674,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1045,11 +1036,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I75"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I76" sqref="I76"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="97" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1105,11 +1096,11 @@
       <c r="C2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="23" t="s">
-        <v>142</v>
+      <c r="E2" s="22" t="s">
+        <v>141</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>13</v>
@@ -1132,7 +1123,7 @@
       <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -1154,7 +1145,7 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="7" t="s">
@@ -1174,13 +1165,15 @@
       <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="7" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
@@ -1192,7 +1185,7 @@
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="7" t="s">
@@ -1202,48 +1195,51 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="7" t="s">
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="14"/>
-    </row>
-    <row r="8" spans="1:9" s="5" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
+      <c r="C7" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="D7" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="E8" s="9"/>
       <c r="F8" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1251,20 +1247,20 @@
         <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1272,20 +1268,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="D10" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1293,20 +1289,20 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1314,153 +1310,152 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E12" s="9"/>
       <c r="F12" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="9"/>
-      <c r="F13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="3" t="s">
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" ht="131.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>44</v>
-      </c>
       <c r="F14" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="F15" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>43</v>
-      </c>
       <c r="F16" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="H17" s="7" t="s">
+    </row>
+    <row r="17" spans="1:9" s="5" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" s="5" customFormat="1" ht="143.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D17" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="F17" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="H17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I18" s="11" t="s">
+    </row>
+    <row r="18" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>60</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1468,19 +1463,19 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D19" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F19" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1488,19 +1483,19 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1508,19 +1503,19 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F21" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1528,19 +1523,19 @@
         <v>9</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F22" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1548,19 +1543,19 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F23" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1568,19 +1563,19 @@
         <v>9</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="4" t="s">
-        <v>56</v>
-      </c>
       <c r="F24" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1588,66 +1583,66 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="F25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" s="6" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="F26" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="12"/>
+      <c r="H26" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" s="6" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="I27" s="15" t="s">
+      <c r="F27" s="7" t="s">
         <v>60</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1655,19 +1650,19 @@
         <v>9</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D28" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1675,19 +1670,19 @@
         <v>9</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D29" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1695,19 +1690,19 @@
         <v>9</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1715,19 +1710,19 @@
         <v>9</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D31" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1735,19 +1730,19 @@
         <v>9</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C32" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D32" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1755,19 +1750,19 @@
         <v>9</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="12" t="s">
-        <v>78</v>
-      </c>
       <c r="D33" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -1775,273 +1770,274 @@
         <v>9</v>
       </c>
       <c r="B34" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="D34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" s="4" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A35" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F35" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D34" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="7" t="s">
+      <c r="G35" s="15"/>
+      <c r="H35" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" s="16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="18"/>
+      <c r="F36" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="I36" s="18"/>
+    </row>
+    <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E37" s="18"/>
+      <c r="F37" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" s="18"/>
+    </row>
+    <row r="38" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G38" s="18"/>
+      <c r="H38" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="I38" s="18"/>
+    </row>
+    <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="18"/>
+    </row>
+    <row r="40" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="18"/>
+      <c r="F40" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G40" s="18"/>
+      <c r="H40" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="I40" s="18"/>
+    </row>
+    <row r="41" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D41" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41" s="18"/>
+      <c r="F41" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G41" s="18"/>
+      <c r="H41" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="I41" s="18"/>
+    </row>
+    <row r="42" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42" s="18"/>
+      <c r="F42" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="18"/>
+      <c r="H42" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H34" s="7" t="s">
+      <c r="I42" s="18"/>
+    </row>
+    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E43" s="18"/>
+      <c r="F43" s="19" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="G43" s="18"/>
+      <c r="H43" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="H35" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="4" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C36" s="16" t="s">
+      <c r="I43" s="18"/>
+    </row>
+    <row r="44" spans="1:9" s="6" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D36" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="G36" s="16"/>
-      <c r="H36" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C37" s="16" t="s">
+      <c r="E44" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D37" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" s="19"/>
-      <c r="F37" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="G37" s="19"/>
-      <c r="H37" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="I37" s="19"/>
-    </row>
-    <row r="38" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E38" s="19"/>
-      <c r="F38" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G38" s="19"/>
-      <c r="H38" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="I38" s="19"/>
-    </row>
-    <row r="39" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E39" s="19"/>
-      <c r="F39" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G39" s="19"/>
-      <c r="H39" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="I39" s="19"/>
-    </row>
-    <row r="40" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E40" s="19"/>
-      <c r="F40" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="G40" s="19"/>
-      <c r="H40" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="I40" s="19"/>
-    </row>
-    <row r="41" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C41" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E41" s="19"/>
-      <c r="F41" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" s="19"/>
-      <c r="H41" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="I41" s="19"/>
-    </row>
-    <row r="42" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C42" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E42" s="19"/>
-      <c r="F42" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G42" s="19"/>
-      <c r="H42" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" s="19"/>
-    </row>
-    <row r="43" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C43" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E43" s="19"/>
-      <c r="F43" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="G43" s="19"/>
-      <c r="H43" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="I43" s="19"/>
-    </row>
-    <row r="44" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="C44" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" s="19"/>
-      <c r="F44" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G44" s="19"/>
-      <c r="H44" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I44" s="19"/>
-    </row>
-    <row r="45" spans="1:9" s="6" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="E45" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>84</v>
+      <c r="F45" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="I45" s="7"/>
     </row>
@@ -2050,19 +2046,19 @@
         <v>9</v>
       </c>
       <c r="B46" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D46" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="I46" s="7"/>
     </row>
@@ -2071,114 +2067,115 @@
         <v>9</v>
       </c>
       <c r="B47" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="D47" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D48" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H48" s="7" t="s">
+    <row r="48" spans="1:9" s="4" customFormat="1" ht="203" x14ac:dyDescent="0.35">
+      <c r="A48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" s="4" customFormat="1" ht="203" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="C48" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="C49" s="10" t="s">
+      <c r="D48" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D49" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="G48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="6" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A49" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E49" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="6" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="F49" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I49" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="D50" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>144</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="E50" s="12"/>
       <c r="F50" s="7" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="I50" s="7" t="s">
-        <v>101</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C51" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="D51" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E51" s="12"/>
       <c r="F51" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="I51" s="7"/>
     </row>
@@ -2187,20 +2184,20 @@
         <v>9</v>
       </c>
       <c r="B52" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="D52" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E52" s="12"/>
       <c r="F52" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I52" s="7"/>
     </row>
@@ -2209,69 +2206,67 @@
         <v>9</v>
       </c>
       <c r="B53" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C53" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="D53" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E53" s="12"/>
       <c r="F53" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D54" s="6" t="s">
+    <row r="54" spans="1:9" s="4" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E54" s="12"/>
-      <c r="F54" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="I54" s="7"/>
-    </row>
-    <row r="55" spans="1:9" s="4" customFormat="1" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="H54" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B55" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C55" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C55" s="9" t="s">
+      <c r="D55" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="E55" s="5" t="s">
-        <v>144</v>
-      </c>
       <c r="F55" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="I55" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="56" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2279,19 +2274,19 @@
         <v>9</v>
       </c>
       <c r="B56" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C56" s="9" t="s">
+      <c r="D56" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D56" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F56" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2299,19 +2294,19 @@
         <v>9</v>
       </c>
       <c r="B57" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C57" s="9" t="s">
+      <c r="D57" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F57" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="58" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2319,85 +2314,85 @@
         <v>9</v>
       </c>
       <c r="B58" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="D58" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="F58" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F59" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H59" s="3" t="s">
+    </row>
+    <row r="59" spans="1:9" s="6" customFormat="1" ht="203" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" s="6" customFormat="1" ht="203" x14ac:dyDescent="0.35">
+      <c r="C59" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B60" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C60" s="13" t="s">
+      <c r="D60" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D60" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>147</v>
-      </c>
       <c r="F60" s="7" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H60" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="I60" s="7" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="61" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B61" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C61" s="13" t="s">
+      <c r="D61" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>112</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>116</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -2405,85 +2400,85 @@
         <v>9</v>
       </c>
       <c r="B62" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C62" s="13" t="s">
+      <c r="D62" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="F62" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" s="4" customFormat="1" ht="203" x14ac:dyDescent="0.35">
+      <c r="A63" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F62" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C63" s="13" t="s">
+      <c r="H63" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="D63" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="H63" s="7" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" s="4" customFormat="1" ht="203" x14ac:dyDescent="0.35">
-      <c r="A64" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>147</v>
-      </c>
       <c r="F64" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H64" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="I64" s="3" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="65" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B65" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>146</v>
-      </c>
       <c r="D65" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>116</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -2491,42 +2486,46 @@
         <v>9</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="C66" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>146</v>
-      </c>
       <c r="D66" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="F67" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H67" s="3" t="s">
+    </row>
+    <row r="67" spans="1:9" s="6" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E67" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="F67" s="7" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" s="6" customFormat="1" ht="188.5" x14ac:dyDescent="0.35">
+      <c r="H67" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I67" s="7"/>
+    </row>
+    <row r="68" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="6" t="s">
         <v>9</v>
       </c>
@@ -2539,16 +2538,12 @@
       <c r="D68" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E68" s="12" t="s">
-        <v>148</v>
-      </c>
       <c r="F68" s="7" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H68" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="I68" s="7"/>
     </row>
     <row r="69" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="6" t="s">
@@ -2567,7 +2562,7 @@
         <v>124</v>
       </c>
       <c r="H69" s="7" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
@@ -2584,293 +2579,273 @@
         <v>11</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H70" s="7" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="H71" s="7" t="s">
+    </row>
+    <row r="71" spans="1:9" s="4" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="A71" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" s="4" customFormat="1" ht="159.5" x14ac:dyDescent="0.35">
+      <c r="C71" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E71" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H71" s="3"/>
+      <c r="I71" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B72" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C72" s="10" t="s">
-        <v>130</v>
-      </c>
       <c r="D72" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="E72" s="5" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="H72" s="3"/>
-      <c r="I72" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F73" s="3" t="s">
+    </row>
+    <row r="73" spans="1:9" s="6" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A73" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="G73" s="3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" s="6" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A74" s="6" t="s">
+      <c r="B73" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C73" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C74" s="13" t="s">
+      <c r="D73" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="D74" s="22" t="s">
+      <c r="E73" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F73" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="E74" s="12" t="s">
+      <c r="G73" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H73" s="7"/>
+      <c r="I73" s="7"/>
+    </row>
+    <row r="74" spans="1:9" s="4" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A74" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E74" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F74" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="G74" s="7" t="s">
+      <c r="F74" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="H74" s="7"/>
-      <c r="I74" s="7"/>
-    </row>
-    <row r="75" spans="1:9" s="4" customFormat="1" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="C75" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="E75" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="F75" s="3" t="s">
+      <c r="G74" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="G75" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H75" s="3"/>
-      <c r="I75" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A35 A45:A123" xr:uid="{9736B45D-7062-4DAC-A85D-EB722845F5A7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A44:A122 A2:A34" xr:uid="{9736B45D-7062-4DAC-A85D-EB722845F5A7}">
       <formula1>"Building,Gate,Roadside,Residential,Infrastructure,Facilities,Car park"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{24E6D53B-CAEC-484B-B7EB-20A312283854}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{417E5000-E30A-45AD-9F2D-FB64BD00B370}"/>
-    <hyperlink ref="H8" r:id="rId3" xr:uid="{4604BE85-81E5-4753-9E60-F5DA42D2BA9B}"/>
-    <hyperlink ref="H9" r:id="rId4" xr:uid="{EF1AAAF2-800C-46C7-9F0E-FC1D5979C49F}"/>
-    <hyperlink ref="F9" r:id="rId5" xr:uid="{AC21C07F-A724-41F6-B6DE-D3869519B2E2}"/>
-    <hyperlink ref="H10" r:id="rId6" xr:uid="{E2E19A25-0B7B-482D-97E5-228CE56E7D68}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{2F5B1D27-38C4-406C-B8C1-5063D6FBE68A}"/>
-    <hyperlink ref="H11" r:id="rId8" xr:uid="{4703C83E-219B-40B8-923F-8FE9DBD93155}"/>
-    <hyperlink ref="F11" r:id="rId9" xr:uid="{EE9A5CC7-FBCD-49B2-8554-244E350DF9C5}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{DF1AE59C-BE04-4E8B-8C3B-81938D9570F1}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{AEC6DD62-55A6-4CFD-900A-95033F9E43D3}"/>
-    <hyperlink ref="F14" r:id="rId12" xr:uid="{8B26FE38-61D8-4A49-8052-B9262A966DAF}"/>
-    <hyperlink ref="H14" r:id="rId13" xr:uid="{BD76390B-8161-4577-88F8-AB1343ED085F}"/>
-    <hyperlink ref="H15" r:id="rId14" xr:uid="{8AE055D8-8B9C-4CD8-A949-8FCE50ACD393}"/>
-    <hyperlink ref="H16" r:id="rId15" xr:uid="{E089225E-EF09-4ED2-9CD1-AFA4C167D9F2}"/>
-    <hyperlink ref="F16" r:id="rId16" xr:uid="{0FD6D2D1-B3D3-49FC-B497-937721745CE2}"/>
-    <hyperlink ref="H17" r:id="rId17" xr:uid="{231A3A26-FD3F-4E85-9459-1A6118E9F7B2}"/>
-    <hyperlink ref="F17" r:id="rId18" xr:uid="{115026A3-C1B5-4A37-8164-D48E3B7D5988}"/>
-    <hyperlink ref="H18" r:id="rId19" xr:uid="{1B011347-CA4C-49AB-AEB6-7AB125CCEBAE}"/>
-    <hyperlink ref="F18" r:id="rId20" xr:uid="{EB1AA3E6-C0BF-43E3-9964-6E5A49FF86F6}"/>
-    <hyperlink ref="H19" r:id="rId21" xr:uid="{5A0BCFF5-7FB7-4433-A696-FCCA9E90E954}"/>
-    <hyperlink ref="F19" r:id="rId22" xr:uid="{4D8BCA38-F689-4A3C-A0B9-41A6A56CDC5F}"/>
-    <hyperlink ref="H20" r:id="rId23" xr:uid="{CD0727F9-235F-495F-88B7-906B1A943C76}"/>
-    <hyperlink ref="F20" r:id="rId24" xr:uid="{568AB699-3E66-4328-B6FD-EA8B5D8EE673}"/>
-    <hyperlink ref="F21" r:id="rId25" xr:uid="{44751EA9-F566-4BD8-A075-CE4AFD941756}"/>
-    <hyperlink ref="H21" r:id="rId26" xr:uid="{2390F596-420E-4954-8726-4D53C6FBA00E}"/>
-    <hyperlink ref="H22" r:id="rId27" xr:uid="{DF90AED7-64C9-4F19-AD46-6C4DA5BCAFC5}"/>
-    <hyperlink ref="F22" r:id="rId28" xr:uid="{4E2672F0-2750-4C49-913A-3041DB8A3481}"/>
-    <hyperlink ref="H23" r:id="rId29" xr:uid="{8CCAE363-0E2E-4541-A3A1-A0F364C3D6C5}"/>
-    <hyperlink ref="F23" r:id="rId30" xr:uid="{888FDB25-FE4B-4B54-8179-79AAD6549404}"/>
-    <hyperlink ref="H24" r:id="rId31" xr:uid="{D7B879A0-DD7F-444C-A021-604FA0196D39}"/>
-    <hyperlink ref="F24" r:id="rId32" xr:uid="{7F2BC20C-4D8E-4B79-AD8B-DB628A9BD9C0}"/>
-    <hyperlink ref="H25" r:id="rId33" xr:uid="{FF153672-019D-441D-A8E6-1802A28CF545}"/>
-    <hyperlink ref="F25" r:id="rId34" xr:uid="{C45A4769-153E-4F68-B5D0-1CD079FED3CB}"/>
-    <hyperlink ref="H26" r:id="rId35" xr:uid="{E14A6E1E-6E52-4505-A314-B1FF69CD0812}"/>
-    <hyperlink ref="F26" r:id="rId36" xr:uid="{4D2FD714-A8D8-416D-AF80-3849F636456B}"/>
-    <hyperlink ref="I8" r:id="rId37" xr:uid="{9C308DB7-28B0-4378-A49A-6D3CFA7D9F88}"/>
-    <hyperlink ref="I14" r:id="rId38" xr:uid="{ACB5E988-5987-4ADE-A0B3-09862D73BAE3}"/>
-    <hyperlink ref="I18" r:id="rId39" xr:uid="{029DA403-B2F4-4028-AF57-0333D6D0DB70}"/>
-    <hyperlink ref="H45" r:id="rId40" xr:uid="{52F0B1FA-B98F-4D8C-B740-2F784CB4C4A6}"/>
-    <hyperlink ref="F46" r:id="rId41" xr:uid="{8470C291-8379-4B8C-BA0E-6A7396A5A2FA}"/>
-    <hyperlink ref="F47" r:id="rId42" xr:uid="{2917CDAF-20FD-469A-AE0C-40C818C9AE14}"/>
-    <hyperlink ref="F48" r:id="rId43" xr:uid="{C38D2B17-B43B-4365-AD59-55B24F7B4307}"/>
-    <hyperlink ref="H46" r:id="rId44" xr:uid="{63E1A31A-A6F6-421F-AD17-CB9ABB15FC5F}"/>
-    <hyperlink ref="H47" r:id="rId45" xr:uid="{09609C44-CDE9-402D-AF45-5128BF82D372}"/>
-    <hyperlink ref="H48" r:id="rId46" xr:uid="{4430CD17-2694-4842-892C-13E21D0C61F4}"/>
-    <hyperlink ref="I55" r:id="rId47" xr:uid="{6D49D4A3-786A-4EC5-94FE-0997B6664D39}"/>
-    <hyperlink ref="F55" r:id="rId48" xr:uid="{F43D753E-1AD6-41C6-8A3C-EBEF895FF438}"/>
-    <hyperlink ref="F56" r:id="rId49" xr:uid="{02858C8C-FE2A-4F44-BBD0-B29092530136}"/>
-    <hyperlink ref="F57" r:id="rId50" xr:uid="{11EB0179-2AA7-4879-825F-DA6B24DF204A}"/>
-    <hyperlink ref="F58" r:id="rId51" xr:uid="{F9986349-99E3-45EA-85F9-4C3D1C71BD5A}"/>
-    <hyperlink ref="F59" r:id="rId52" xr:uid="{CDAC31A9-9C44-48B0-9EBF-B7F1AC432C62}"/>
-    <hyperlink ref="H55" r:id="rId53" xr:uid="{CB8E7B01-28C7-43DA-9FC2-C4AE16CA89C3}"/>
-    <hyperlink ref="H56" r:id="rId54" xr:uid="{9E77C1FF-0D95-4DC8-B679-9AB655636DC0}"/>
-    <hyperlink ref="H57" r:id="rId55" xr:uid="{EE54DF95-0159-424B-BEAE-A82E3C052C0D}"/>
-    <hyperlink ref="H58" r:id="rId56" xr:uid="{C06FF6F3-B4AE-419F-BCEC-0BBC4A27DD30}"/>
-    <hyperlink ref="H59" r:id="rId57" xr:uid="{A24AF1C9-4547-4ABD-B411-43E9BA5B1517}"/>
-    <hyperlink ref="F60" r:id="rId58" xr:uid="{B36457CF-3365-46B5-A2D6-F61DE89E15BB}"/>
-    <hyperlink ref="F61" r:id="rId59" xr:uid="{6F332AFE-1AC2-44A0-BFBA-C6DF656FD5DC}"/>
-    <hyperlink ref="F62" r:id="rId60" xr:uid="{C11473F8-5274-45B1-B350-9A009CF2C41F}"/>
-    <hyperlink ref="F63" r:id="rId61" xr:uid="{460769EA-6A96-4305-9857-B47C9B356188}"/>
-    <hyperlink ref="H60" r:id="rId62" xr:uid="{B5613E81-921D-4E4D-A6E6-C25ECCCA3ECB}"/>
-    <hyperlink ref="H61" r:id="rId63" xr:uid="{9572D3F6-B5E2-40DF-B137-A92C84E9F969}"/>
-    <hyperlink ref="H62" r:id="rId64" xr:uid="{72F42F87-28AE-4686-942C-CDC3A48F398A}"/>
-    <hyperlink ref="H63" r:id="rId65" xr:uid="{F66545C5-F56F-4AEC-BB4D-9A56BC969BCD}"/>
-    <hyperlink ref="F68" r:id="rId66" xr:uid="{34C37236-164F-48F6-8CCC-1AF2724666BE}"/>
-    <hyperlink ref="F69" r:id="rId67" xr:uid="{8A8E72C3-8B77-4AF7-82BA-BB87B6F52908}"/>
-    <hyperlink ref="F70" r:id="rId68" xr:uid="{9B32B263-3DBF-4EDB-B073-8D62B865824F}"/>
-    <hyperlink ref="F71" r:id="rId69" xr:uid="{969301CC-897F-4C94-8E0F-390ADD60B87A}"/>
-    <hyperlink ref="H68" r:id="rId70" xr:uid="{288A6B3C-906E-43B9-858C-B2C5F91E6BC9}"/>
-    <hyperlink ref="H69" r:id="rId71" xr:uid="{D372FFCC-A102-4184-A33E-B05DA7E47275}"/>
-    <hyperlink ref="H70" r:id="rId72" xr:uid="{709808F6-B5F0-4214-B2F9-4C6B490367A9}"/>
-    <hyperlink ref="H71" r:id="rId73" xr:uid="{5183A407-4599-4593-B518-FEC71CACED7A}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{417E5000-E30A-45AD-9F2D-FB64BD00B370}"/>
+    <hyperlink ref="H7" r:id="rId3" xr:uid="{4604BE85-81E5-4753-9E60-F5DA42D2BA9B}"/>
+    <hyperlink ref="H8" r:id="rId4" xr:uid="{EF1AAAF2-800C-46C7-9F0E-FC1D5979C49F}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{AC21C07F-A724-41F6-B6DE-D3869519B2E2}"/>
+    <hyperlink ref="H9" r:id="rId6" xr:uid="{E2E19A25-0B7B-482D-97E5-228CE56E7D68}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{2F5B1D27-38C4-406C-B8C1-5063D6FBE68A}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{4703C83E-219B-40B8-923F-8FE9DBD93155}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{EE9A5CC7-FBCD-49B2-8554-244E350DF9C5}"/>
+    <hyperlink ref="H11" r:id="rId10" xr:uid="{DF1AE59C-BE04-4E8B-8C3B-81938D9570F1}"/>
+    <hyperlink ref="F11" r:id="rId11" xr:uid="{AEC6DD62-55A6-4CFD-900A-95033F9E43D3}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{8B26FE38-61D8-4A49-8052-B9262A966DAF}"/>
+    <hyperlink ref="H13" r:id="rId13" xr:uid="{BD76390B-8161-4577-88F8-AB1343ED085F}"/>
+    <hyperlink ref="H14" r:id="rId14" xr:uid="{8AE055D8-8B9C-4CD8-A949-8FCE50ACD393}"/>
+    <hyperlink ref="H15" r:id="rId15" xr:uid="{E089225E-EF09-4ED2-9CD1-AFA4C167D9F2}"/>
+    <hyperlink ref="F15" r:id="rId16" xr:uid="{0FD6D2D1-B3D3-49FC-B497-937721745CE2}"/>
+    <hyperlink ref="H16" r:id="rId17" xr:uid="{231A3A26-FD3F-4E85-9459-1A6118E9F7B2}"/>
+    <hyperlink ref="F16" r:id="rId18" xr:uid="{115026A3-C1B5-4A37-8164-D48E3B7D5988}"/>
+    <hyperlink ref="H17" r:id="rId19" xr:uid="{1B011347-CA4C-49AB-AEB6-7AB125CCEBAE}"/>
+    <hyperlink ref="F17" r:id="rId20" xr:uid="{EB1AA3E6-C0BF-43E3-9964-6E5A49FF86F6}"/>
+    <hyperlink ref="H18" r:id="rId21" xr:uid="{5A0BCFF5-7FB7-4433-A696-FCCA9E90E954}"/>
+    <hyperlink ref="F18" r:id="rId22" xr:uid="{4D8BCA38-F689-4A3C-A0B9-41A6A56CDC5F}"/>
+    <hyperlink ref="H19" r:id="rId23" xr:uid="{CD0727F9-235F-495F-88B7-906B1A943C76}"/>
+    <hyperlink ref="F19" r:id="rId24" xr:uid="{568AB699-3E66-4328-B6FD-EA8B5D8EE673}"/>
+    <hyperlink ref="F20" r:id="rId25" xr:uid="{44751EA9-F566-4BD8-A075-CE4AFD941756}"/>
+    <hyperlink ref="H20" r:id="rId26" xr:uid="{2390F596-420E-4954-8726-4D53C6FBA00E}"/>
+    <hyperlink ref="H21" r:id="rId27" xr:uid="{DF90AED7-64C9-4F19-AD46-6C4DA5BCAFC5}"/>
+    <hyperlink ref="F21" r:id="rId28" xr:uid="{4E2672F0-2750-4C49-913A-3041DB8A3481}"/>
+    <hyperlink ref="H22" r:id="rId29" xr:uid="{8CCAE363-0E2E-4541-A3A1-A0F364C3D6C5}"/>
+    <hyperlink ref="F22" r:id="rId30" xr:uid="{888FDB25-FE4B-4B54-8179-79AAD6549404}"/>
+    <hyperlink ref="H23" r:id="rId31" xr:uid="{D7B879A0-DD7F-444C-A021-604FA0196D39}"/>
+    <hyperlink ref="F23" r:id="rId32" xr:uid="{7F2BC20C-4D8E-4B79-AD8B-DB628A9BD9C0}"/>
+    <hyperlink ref="H24" r:id="rId33" xr:uid="{FF153672-019D-441D-A8E6-1802A28CF545}"/>
+    <hyperlink ref="F24" r:id="rId34" xr:uid="{C45A4769-153E-4F68-B5D0-1CD079FED3CB}"/>
+    <hyperlink ref="H25" r:id="rId35" xr:uid="{E14A6E1E-6E52-4505-A314-B1FF69CD0812}"/>
+    <hyperlink ref="F25" r:id="rId36" xr:uid="{4D2FD714-A8D8-416D-AF80-3849F636456B}"/>
+    <hyperlink ref="I7" r:id="rId37" xr:uid="{9C308DB7-28B0-4378-A49A-6D3CFA7D9F88}"/>
+    <hyperlink ref="I13" r:id="rId38" xr:uid="{ACB5E988-5987-4ADE-A0B3-09862D73BAE3}"/>
+    <hyperlink ref="I17" r:id="rId39" xr:uid="{029DA403-B2F4-4028-AF57-0333D6D0DB70}"/>
+    <hyperlink ref="H44" r:id="rId40" xr:uid="{52F0B1FA-B98F-4D8C-B740-2F784CB4C4A6}"/>
+    <hyperlink ref="F45" r:id="rId41" xr:uid="{8470C291-8379-4B8C-BA0E-6A7396A5A2FA}"/>
+    <hyperlink ref="F46" r:id="rId42" xr:uid="{2917CDAF-20FD-469A-AE0C-40C818C9AE14}"/>
+    <hyperlink ref="F47" r:id="rId43" xr:uid="{C38D2B17-B43B-4365-AD59-55B24F7B4307}"/>
+    <hyperlink ref="H45" r:id="rId44" xr:uid="{63E1A31A-A6F6-421F-AD17-CB9ABB15FC5F}"/>
+    <hyperlink ref="H46" r:id="rId45" xr:uid="{09609C44-CDE9-402D-AF45-5128BF82D372}"/>
+    <hyperlink ref="H47" r:id="rId46" xr:uid="{4430CD17-2694-4842-892C-13E21D0C61F4}"/>
+    <hyperlink ref="I54" r:id="rId47" xr:uid="{6D49D4A3-786A-4EC5-94FE-0997B6664D39}"/>
+    <hyperlink ref="F54" r:id="rId48" xr:uid="{F43D753E-1AD6-41C6-8A3C-EBEF895FF438}"/>
+    <hyperlink ref="F55" r:id="rId49" xr:uid="{02858C8C-FE2A-4F44-BBD0-B29092530136}"/>
+    <hyperlink ref="F56" r:id="rId50" xr:uid="{11EB0179-2AA7-4879-825F-DA6B24DF204A}"/>
+    <hyperlink ref="F57" r:id="rId51" xr:uid="{F9986349-99E3-45EA-85F9-4C3D1C71BD5A}"/>
+    <hyperlink ref="F58" r:id="rId52" xr:uid="{CDAC31A9-9C44-48B0-9EBF-B7F1AC432C62}"/>
+    <hyperlink ref="H54" r:id="rId53" xr:uid="{CB8E7B01-28C7-43DA-9FC2-C4AE16CA89C3}"/>
+    <hyperlink ref="H55" r:id="rId54" xr:uid="{9E77C1FF-0D95-4DC8-B679-9AB655636DC0}"/>
+    <hyperlink ref="H56" r:id="rId55" xr:uid="{EE54DF95-0159-424B-BEAE-A82E3C052C0D}"/>
+    <hyperlink ref="H57" r:id="rId56" xr:uid="{C06FF6F3-B4AE-419F-BCEC-0BBC4A27DD30}"/>
+    <hyperlink ref="H58" r:id="rId57" xr:uid="{A24AF1C9-4547-4ABD-B411-43E9BA5B1517}"/>
+    <hyperlink ref="F59" r:id="rId58" xr:uid="{B36457CF-3365-46B5-A2D6-F61DE89E15BB}"/>
+    <hyperlink ref="F60" r:id="rId59" xr:uid="{6F332AFE-1AC2-44A0-BFBA-C6DF656FD5DC}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{C11473F8-5274-45B1-B350-9A009CF2C41F}"/>
+    <hyperlink ref="F62" r:id="rId61" xr:uid="{460769EA-6A96-4305-9857-B47C9B356188}"/>
+    <hyperlink ref="H59" r:id="rId62" xr:uid="{B5613E81-921D-4E4D-A6E6-C25ECCCA3ECB}"/>
+    <hyperlink ref="H60" r:id="rId63" xr:uid="{9572D3F6-B5E2-40DF-B137-A92C84E9F969}"/>
+    <hyperlink ref="H61" r:id="rId64" xr:uid="{72F42F87-28AE-4686-942C-CDC3A48F398A}"/>
+    <hyperlink ref="H62" r:id="rId65" xr:uid="{F66545C5-F56F-4AEC-BB4D-9A56BC969BCD}"/>
+    <hyperlink ref="F67" r:id="rId66" xr:uid="{34C37236-164F-48F6-8CCC-1AF2724666BE}"/>
+    <hyperlink ref="F68" r:id="rId67" xr:uid="{8A8E72C3-8B77-4AF7-82BA-BB87B6F52908}"/>
+    <hyperlink ref="F69" r:id="rId68" xr:uid="{9B32B263-3DBF-4EDB-B073-8D62B865824F}"/>
+    <hyperlink ref="F70" r:id="rId69" xr:uid="{969301CC-897F-4C94-8E0F-390ADD60B87A}"/>
+    <hyperlink ref="H67" r:id="rId70" xr:uid="{288A6B3C-906E-43B9-858C-B2C5F91E6BC9}"/>
+    <hyperlink ref="H68" r:id="rId71" xr:uid="{D372FFCC-A102-4184-A33E-B05DA7E47275}"/>
+    <hyperlink ref="H69" r:id="rId72" xr:uid="{709808F6-B5F0-4214-B2F9-4C6B490367A9}"/>
+    <hyperlink ref="H70" r:id="rId73" xr:uid="{5183A407-4599-4593-B518-FEC71CACED7A}"/>
     <hyperlink ref="G2" r:id="rId74" xr:uid="{64B6B160-E142-47A4-8515-6489FA2E3C0B}"/>
     <hyperlink ref="F3" r:id="rId75" xr:uid="{C316479B-7E66-4679-B953-93F4B6F22388}"/>
     <hyperlink ref="F4" r:id="rId76" xr:uid="{190EBED5-F8A3-45F3-8859-54CC9EB42433}"/>
     <hyperlink ref="F5" r:id="rId77" xr:uid="{A899F343-08B1-4455-AB70-9304EF166B1F}"/>
     <hyperlink ref="F6" r:id="rId78" xr:uid="{F672369F-9E8E-44FC-B04B-A42F1ED0A3B4}"/>
-    <hyperlink ref="F7" r:id="rId79" xr:uid="{AD8418A2-B3E6-4E4E-9747-D99C9113B71A}"/>
-    <hyperlink ref="G6" r:id="rId80" xr:uid="{CEEEAEB1-721B-47CC-AA4B-12D2602530C9}"/>
-    <hyperlink ref="G3" r:id="rId81" xr:uid="{CF4C380C-ADD0-48C2-BB8D-34C0539AC48B}"/>
-    <hyperlink ref="G4" r:id="rId82" xr:uid="{98C36019-655D-49F7-BA2C-972982D8C342}"/>
-    <hyperlink ref="G74" r:id="rId83" xr:uid="{F0AFFE47-6AD0-474A-8FD0-4D46555C02A4}"/>
-    <hyperlink ref="F74" r:id="rId84" xr:uid="{0972361D-5913-4A0D-9047-A77F2CD1E100}"/>
-    <hyperlink ref="G75" r:id="rId85" xr:uid="{2751D7C5-20B5-4933-9993-9F3F996E42C3}"/>
-    <hyperlink ref="F75" r:id="rId86" xr:uid="{78E92A8F-FB4A-4550-815D-1DAEAB1D868E}"/>
-    <hyperlink ref="F72" r:id="rId87" xr:uid="{2729D69E-FCCC-4F0C-96DE-5DEB8F3EB622}"/>
-    <hyperlink ref="F73" r:id="rId88" xr:uid="{2AB284D6-1083-401A-8423-EEF28BF1BE7F}"/>
-    <hyperlink ref="G72" r:id="rId89" xr:uid="{6432ED58-5591-4EB4-9718-338A715BD6CA}"/>
-    <hyperlink ref="G73" r:id="rId90" xr:uid="{DD18888A-34DD-4E33-97AE-6097C5486ABA}"/>
-    <hyperlink ref="I60" r:id="rId91" xr:uid="{750CE46C-47E5-4E63-AC94-8CFF9859A677}"/>
-    <hyperlink ref="I72" r:id="rId92" xr:uid="{83605291-05F2-459F-AFBF-924565F64BEF}"/>
-    <hyperlink ref="F49" r:id="rId93" xr:uid="{7737C373-381D-47EB-BDCD-CF6915E07F76}"/>
-    <hyperlink ref="G49" r:id="rId94" xr:uid="{C70BAE64-B056-49DE-B34F-066E5384C0DD}"/>
-    <hyperlink ref="I49" r:id="rId95" xr:uid="{A140E166-FEF4-46D9-89B0-CE40BB1F7C94}"/>
-    <hyperlink ref="F15" r:id="rId96" xr:uid="{CB2F5134-AA02-47CD-B84D-034E9F9DDC6D}"/>
-    <hyperlink ref="F13" r:id="rId97" xr:uid="{59F2BA44-7C2E-49A2-90C0-D2FD5E999392}"/>
-    <hyperlink ref="H13" r:id="rId98" xr:uid="{45C5CF9F-DA53-4710-B3A1-AA78FB3FBB42}"/>
-    <hyperlink ref="I2" r:id="rId99" xr:uid="{4A62B64E-4355-43C1-9C22-23230A1DF106}"/>
-    <hyperlink ref="H27" r:id="rId100" xr:uid="{380B04F1-CF24-4CC0-88FC-7C34CA04C80A}"/>
-    <hyperlink ref="F27" r:id="rId101" xr:uid="{1F24137D-5CC7-471E-8CBD-85B48E8ED650}"/>
-    <hyperlink ref="H28" r:id="rId102" xr:uid="{B0A4D6F9-B171-4DF3-A6EE-5E1DE84F2CF1}"/>
-    <hyperlink ref="F28" r:id="rId103" xr:uid="{E926C98B-F866-4808-A215-93263BEBF62E}"/>
-    <hyperlink ref="H29" r:id="rId104" xr:uid="{E6BEEB6F-AF5E-4CC6-A1D3-6E921D2B1E6B}"/>
-    <hyperlink ref="F29" r:id="rId105" xr:uid="{DD925CF6-B220-4921-AFA1-916ADBF97DCF}"/>
-    <hyperlink ref="F30" r:id="rId106" xr:uid="{4AD54800-0C7E-4170-9BA9-257D2F4C6180}"/>
-    <hyperlink ref="H30" r:id="rId107" xr:uid="{E01D2C2B-477D-4884-8369-61F4858EB7F3}"/>
-    <hyperlink ref="H31" r:id="rId108" xr:uid="{2AAC270E-3755-4B8E-963D-0A96EA517BAC}"/>
-    <hyperlink ref="F31" r:id="rId109" xr:uid="{8B9AE03B-D434-4682-9C1F-1551A97DDA7B}"/>
-    <hyperlink ref="H32" r:id="rId110" xr:uid="{8CD1E31D-85F5-4B98-80B2-59A71C1BE85F}"/>
-    <hyperlink ref="F32" r:id="rId111" xr:uid="{900829DE-2875-4577-A14E-0EA235AF27F6}"/>
-    <hyperlink ref="H33" r:id="rId112" xr:uid="{251E2EF6-5AFA-42B7-A424-18DFD48BDBCD}"/>
-    <hyperlink ref="F33" r:id="rId113" xr:uid="{C45A3607-879F-4BEE-974D-A0C89DDD1E68}"/>
-    <hyperlink ref="H34" r:id="rId114" xr:uid="{EE1B61EA-9EBD-4B97-A741-4FDBF6E56FF6}"/>
-    <hyperlink ref="F34" r:id="rId115" xr:uid="{9DD3E1D0-55D4-49EC-83B0-CEF54794AC90}"/>
-    <hyperlink ref="H35" r:id="rId116" xr:uid="{ECBA104D-DDAD-47FC-8612-2FC77A2E5C87}"/>
-    <hyperlink ref="F35" r:id="rId117" xr:uid="{9C89C383-1F0D-4A42-8F5B-FD844D41BC81}"/>
-    <hyperlink ref="I27" r:id="rId118" xr:uid="{F8EDF862-6C10-40E2-954C-25AE580F5686}"/>
-    <hyperlink ref="F36" r:id="rId119" xr:uid="{5CFD8208-4725-4809-B3F8-9AF4F104B4FB}"/>
-    <hyperlink ref="H36" r:id="rId120" xr:uid="{B074CC72-E371-4F1A-971D-7FD19A5BD6BA}"/>
-    <hyperlink ref="I36" r:id="rId121" xr:uid="{114FA688-1374-423E-A400-DD37C2D0C2DF}"/>
-    <hyperlink ref="F37" r:id="rId122" xr:uid="{9EF4DFF4-C006-4FEC-B059-16FA5834F8A0}"/>
-    <hyperlink ref="H37" r:id="rId123" xr:uid="{FBE69C16-D226-4B96-96FC-F50BDE7E7677}"/>
-    <hyperlink ref="F38" r:id="rId124" xr:uid="{8BA3CAC3-A317-4B22-B977-E8884D38A316}"/>
-    <hyperlink ref="H38" r:id="rId125" xr:uid="{82554320-AA0E-4711-93A5-8AC314E3D3CE}"/>
-    <hyperlink ref="F39" r:id="rId126" xr:uid="{07B8346A-0883-405A-87DF-AC9EE5267B88}"/>
-    <hyperlink ref="H39" r:id="rId127" xr:uid="{6C8D6477-7F76-4C96-A3A1-CF6C8123DD75}"/>
-    <hyperlink ref="F40" r:id="rId128" xr:uid="{6F5E247A-FEC4-4EB6-A40F-AC1E06D8DCCA}"/>
-    <hyperlink ref="H40" r:id="rId129" xr:uid="{6C832E9E-2D29-449A-9D6E-8E51532D5235}"/>
-    <hyperlink ref="F41" r:id="rId130" xr:uid="{B224394C-B9B1-4767-8DD4-D6B9D4E35FC1}"/>
-    <hyperlink ref="H41" r:id="rId131" xr:uid="{6B6DA752-2CC5-4511-9CD0-272C254B35F4}"/>
-    <hyperlink ref="F42" r:id="rId132" xr:uid="{93FB6000-41F7-4F94-AED9-075BD4FBEE5D}"/>
-    <hyperlink ref="H42" r:id="rId133" xr:uid="{2659F134-173B-4BA3-8FA2-87EE84509B47}"/>
-    <hyperlink ref="F43" r:id="rId134" xr:uid="{85A8E1D6-6F60-4FF2-A256-5A2D1938053C}"/>
-    <hyperlink ref="H43" r:id="rId135" xr:uid="{73EF31DC-C06A-49E2-A34A-C3ABE9CED0E8}"/>
-    <hyperlink ref="F44" r:id="rId136" xr:uid="{ACA47DC8-BAE7-486C-9EDF-689620EEF0CD}"/>
-    <hyperlink ref="H44" r:id="rId137" xr:uid="{4F3BFCA6-BB94-454E-8B65-0F82890A6699}"/>
-    <hyperlink ref="F50" r:id="rId138" xr:uid="{3437B6EA-7B80-475A-B126-23F2CE69E3CF}"/>
-    <hyperlink ref="F51" r:id="rId139" xr:uid="{B4F3B46B-F68F-40F9-87D4-417425A3EBD4}"/>
-    <hyperlink ref="F52" r:id="rId140" xr:uid="{0DFE9A38-8E43-417F-938A-EA453016E561}"/>
-    <hyperlink ref="F53" r:id="rId141" xr:uid="{C0A2A5B6-928C-41E9-82F8-7C5B498DA34A}"/>
-    <hyperlink ref="F54" r:id="rId142" xr:uid="{C9D3F6E1-D127-4501-B410-B4F18DAEDCCC}"/>
-    <hyperlink ref="H50" r:id="rId143" xr:uid="{96397BB4-4ABE-46A3-BA73-55A61E61178D}"/>
-    <hyperlink ref="H51" r:id="rId144" xr:uid="{1C3D4B26-7978-445B-BC18-8EE7E8674B3E}"/>
-    <hyperlink ref="H52" r:id="rId145" xr:uid="{DF7A6C78-8ADE-4870-9EBE-1EF5A0235E5F}"/>
-    <hyperlink ref="H53" r:id="rId146" xr:uid="{02D98F1D-B5BD-4BDC-9D9F-7BF30DF2E7A6}"/>
-    <hyperlink ref="H54" r:id="rId147" xr:uid="{12BCA759-FE0B-4D3C-8250-E062728A6FD8}"/>
-    <hyperlink ref="F64" r:id="rId148" xr:uid="{F287F6A3-7EBD-4437-9DEA-6900C419A737}"/>
-    <hyperlink ref="F65" r:id="rId149" xr:uid="{E49D4920-8389-4C3A-90B0-260399FA3A20}"/>
-    <hyperlink ref="F66" r:id="rId150" xr:uid="{F308AE64-CA6C-4B1D-AFEB-DAE8B9EAE70A}"/>
-    <hyperlink ref="F67" r:id="rId151" xr:uid="{05029475-CE13-48E4-8A60-CC62D05E67E0}"/>
-    <hyperlink ref="H64" r:id="rId152" xr:uid="{D6A73AC2-E608-4390-972F-4C00760E5C6D}"/>
-    <hyperlink ref="H65" r:id="rId153" xr:uid="{2F558378-5BC3-4382-8DA2-59949F14D6B3}"/>
-    <hyperlink ref="H66" r:id="rId154" xr:uid="{E01483F8-09F3-4452-BF30-1843E2DAC026}"/>
-    <hyperlink ref="H67" r:id="rId155" xr:uid="{420AE97C-C75D-4654-A5BC-2C6CD52393BE}"/>
-    <hyperlink ref="I64" r:id="rId156" xr:uid="{70DBAC93-6CC4-4257-B3CA-B596B587411B}"/>
+    <hyperlink ref="G6" r:id="rId79" xr:uid="{CEEEAEB1-721B-47CC-AA4B-12D2602530C9}"/>
+    <hyperlink ref="G3" r:id="rId80" xr:uid="{CF4C380C-ADD0-48C2-BB8D-34C0539AC48B}"/>
+    <hyperlink ref="G4" r:id="rId81" xr:uid="{98C36019-655D-49F7-BA2C-972982D8C342}"/>
+    <hyperlink ref="G73" r:id="rId82" xr:uid="{F0AFFE47-6AD0-474A-8FD0-4D46555C02A4}"/>
+    <hyperlink ref="F73" r:id="rId83" xr:uid="{0972361D-5913-4A0D-9047-A77F2CD1E100}"/>
+    <hyperlink ref="G74" r:id="rId84" xr:uid="{2751D7C5-20B5-4933-9993-9F3F996E42C3}"/>
+    <hyperlink ref="F74" r:id="rId85" xr:uid="{78E92A8F-FB4A-4550-815D-1DAEAB1D868E}"/>
+    <hyperlink ref="F71" r:id="rId86" xr:uid="{2729D69E-FCCC-4F0C-96DE-5DEB8F3EB622}"/>
+    <hyperlink ref="F72" r:id="rId87" xr:uid="{2AB284D6-1083-401A-8423-EEF28BF1BE7F}"/>
+    <hyperlink ref="G71" r:id="rId88" xr:uid="{6432ED58-5591-4EB4-9718-338A715BD6CA}"/>
+    <hyperlink ref="G72" r:id="rId89" xr:uid="{DD18888A-34DD-4E33-97AE-6097C5486ABA}"/>
+    <hyperlink ref="I59" r:id="rId90" xr:uid="{750CE46C-47E5-4E63-AC94-8CFF9859A677}"/>
+    <hyperlink ref="I71" r:id="rId91" xr:uid="{83605291-05F2-459F-AFBF-924565F64BEF}"/>
+    <hyperlink ref="F48" r:id="rId92" xr:uid="{7737C373-381D-47EB-BDCD-CF6915E07F76}"/>
+    <hyperlink ref="G48" r:id="rId93" xr:uid="{C70BAE64-B056-49DE-B34F-066E5384C0DD}"/>
+    <hyperlink ref="I48" r:id="rId94" xr:uid="{A140E166-FEF4-46D9-89B0-CE40BB1F7C94}"/>
+    <hyperlink ref="F14" r:id="rId95" xr:uid="{CB2F5134-AA02-47CD-B84D-034E9F9DDC6D}"/>
+    <hyperlink ref="F12" r:id="rId96" xr:uid="{59F2BA44-7C2E-49A2-90C0-D2FD5E999392}"/>
+    <hyperlink ref="H12" r:id="rId97" xr:uid="{45C5CF9F-DA53-4710-B3A1-AA78FB3FBB42}"/>
+    <hyperlink ref="I2" r:id="rId98" xr:uid="{4A62B64E-4355-43C1-9C22-23230A1DF106}"/>
+    <hyperlink ref="H26" r:id="rId99" xr:uid="{380B04F1-CF24-4CC0-88FC-7C34CA04C80A}"/>
+    <hyperlink ref="F26" r:id="rId100" xr:uid="{1F24137D-5CC7-471E-8CBD-85B48E8ED650}"/>
+    <hyperlink ref="H27" r:id="rId101" xr:uid="{B0A4D6F9-B171-4DF3-A6EE-5E1DE84F2CF1}"/>
+    <hyperlink ref="F27" r:id="rId102" xr:uid="{E926C98B-F866-4808-A215-93263BEBF62E}"/>
+    <hyperlink ref="H28" r:id="rId103" xr:uid="{E6BEEB6F-AF5E-4CC6-A1D3-6E921D2B1E6B}"/>
+    <hyperlink ref="F28" r:id="rId104" xr:uid="{DD925CF6-B220-4921-AFA1-916ADBF97DCF}"/>
+    <hyperlink ref="F29" r:id="rId105" xr:uid="{4AD54800-0C7E-4170-9BA9-257D2F4C6180}"/>
+    <hyperlink ref="H29" r:id="rId106" xr:uid="{E01D2C2B-477D-4884-8369-61F4858EB7F3}"/>
+    <hyperlink ref="H30" r:id="rId107" xr:uid="{2AAC270E-3755-4B8E-963D-0A96EA517BAC}"/>
+    <hyperlink ref="F30" r:id="rId108" xr:uid="{8B9AE03B-D434-4682-9C1F-1551A97DDA7B}"/>
+    <hyperlink ref="H31" r:id="rId109" xr:uid="{8CD1E31D-85F5-4B98-80B2-59A71C1BE85F}"/>
+    <hyperlink ref="F31" r:id="rId110" xr:uid="{900829DE-2875-4577-A14E-0EA235AF27F6}"/>
+    <hyperlink ref="H32" r:id="rId111" xr:uid="{251E2EF6-5AFA-42B7-A424-18DFD48BDBCD}"/>
+    <hyperlink ref="F32" r:id="rId112" xr:uid="{C45A3607-879F-4BEE-974D-A0C89DDD1E68}"/>
+    <hyperlink ref="H33" r:id="rId113" xr:uid="{EE1B61EA-9EBD-4B97-A741-4FDBF6E56FF6}"/>
+    <hyperlink ref="F33" r:id="rId114" xr:uid="{9DD3E1D0-55D4-49EC-83B0-CEF54794AC90}"/>
+    <hyperlink ref="H34" r:id="rId115" xr:uid="{ECBA104D-DDAD-47FC-8612-2FC77A2E5C87}"/>
+    <hyperlink ref="F34" r:id="rId116" xr:uid="{9C89C383-1F0D-4A42-8F5B-FD844D41BC81}"/>
+    <hyperlink ref="I26" r:id="rId117" xr:uid="{F8EDF862-6C10-40E2-954C-25AE580F5686}"/>
+    <hyperlink ref="F35" r:id="rId118" xr:uid="{5CFD8208-4725-4809-B3F8-9AF4F104B4FB}"/>
+    <hyperlink ref="H35" r:id="rId119" xr:uid="{B074CC72-E371-4F1A-971D-7FD19A5BD6BA}"/>
+    <hyperlink ref="I35" r:id="rId120" xr:uid="{114FA688-1374-423E-A400-DD37C2D0C2DF}"/>
+    <hyperlink ref="F36" r:id="rId121" xr:uid="{9EF4DFF4-C006-4FEC-B059-16FA5834F8A0}"/>
+    <hyperlink ref="H36" r:id="rId122" xr:uid="{FBE69C16-D226-4B96-96FC-F50BDE7E7677}"/>
+    <hyperlink ref="F37" r:id="rId123" xr:uid="{8BA3CAC3-A317-4B22-B977-E8884D38A316}"/>
+    <hyperlink ref="H37" r:id="rId124" xr:uid="{82554320-AA0E-4711-93A5-8AC314E3D3CE}"/>
+    <hyperlink ref="F38" r:id="rId125" xr:uid="{07B8346A-0883-405A-87DF-AC9EE5267B88}"/>
+    <hyperlink ref="H38" r:id="rId126" xr:uid="{6C8D6477-7F76-4C96-A3A1-CF6C8123DD75}"/>
+    <hyperlink ref="F39" r:id="rId127" xr:uid="{6F5E247A-FEC4-4EB6-A40F-AC1E06D8DCCA}"/>
+    <hyperlink ref="H39" r:id="rId128" xr:uid="{6C832E9E-2D29-449A-9D6E-8E51532D5235}"/>
+    <hyperlink ref="F40" r:id="rId129" xr:uid="{B224394C-B9B1-4767-8DD4-D6B9D4E35FC1}"/>
+    <hyperlink ref="H40" r:id="rId130" xr:uid="{6B6DA752-2CC5-4511-9CD0-272C254B35F4}"/>
+    <hyperlink ref="F41" r:id="rId131" xr:uid="{93FB6000-41F7-4F94-AED9-075BD4FBEE5D}"/>
+    <hyperlink ref="H41" r:id="rId132" xr:uid="{2659F134-173B-4BA3-8FA2-87EE84509B47}"/>
+    <hyperlink ref="F42" r:id="rId133" xr:uid="{85A8E1D6-6F60-4FF2-A256-5A2D1938053C}"/>
+    <hyperlink ref="H42" r:id="rId134" xr:uid="{73EF31DC-C06A-49E2-A34A-C3ABE9CED0E8}"/>
+    <hyperlink ref="F43" r:id="rId135" xr:uid="{ACA47DC8-BAE7-486C-9EDF-689620EEF0CD}"/>
+    <hyperlink ref="H43" r:id="rId136" xr:uid="{4F3BFCA6-BB94-454E-8B65-0F82890A6699}"/>
+    <hyperlink ref="F49" r:id="rId137" xr:uid="{3437B6EA-7B80-475A-B126-23F2CE69E3CF}"/>
+    <hyperlink ref="F50" r:id="rId138" xr:uid="{B4F3B46B-F68F-40F9-87D4-417425A3EBD4}"/>
+    <hyperlink ref="F51" r:id="rId139" xr:uid="{0DFE9A38-8E43-417F-938A-EA453016E561}"/>
+    <hyperlink ref="F52" r:id="rId140" xr:uid="{C0A2A5B6-928C-41E9-82F8-7C5B498DA34A}"/>
+    <hyperlink ref="F53" r:id="rId141" xr:uid="{C9D3F6E1-D127-4501-B410-B4F18DAEDCCC}"/>
+    <hyperlink ref="H49" r:id="rId142" xr:uid="{96397BB4-4ABE-46A3-BA73-55A61E61178D}"/>
+    <hyperlink ref="H50" r:id="rId143" xr:uid="{1C3D4B26-7978-445B-BC18-8EE7E8674B3E}"/>
+    <hyperlink ref="H51" r:id="rId144" xr:uid="{DF7A6C78-8ADE-4870-9EBE-1EF5A0235E5F}"/>
+    <hyperlink ref="H52" r:id="rId145" xr:uid="{02D98F1D-B5BD-4BDC-9D9F-7BF30DF2E7A6}"/>
+    <hyperlink ref="H53" r:id="rId146" xr:uid="{12BCA759-FE0B-4D3C-8250-E062728A6FD8}"/>
+    <hyperlink ref="F63" r:id="rId147" xr:uid="{F287F6A3-7EBD-4437-9DEA-6900C419A737}"/>
+    <hyperlink ref="F64" r:id="rId148" xr:uid="{E49D4920-8389-4C3A-90B0-260399FA3A20}"/>
+    <hyperlink ref="F65" r:id="rId149" xr:uid="{F308AE64-CA6C-4B1D-AFEB-DAE8B9EAE70A}"/>
+    <hyperlink ref="F66" r:id="rId150" xr:uid="{05029475-CE13-48E4-8A60-CC62D05E67E0}"/>
+    <hyperlink ref="H63" r:id="rId151" xr:uid="{D6A73AC2-E608-4390-972F-4C00760E5C6D}"/>
+    <hyperlink ref="H64" r:id="rId152" xr:uid="{2F558378-5BC3-4382-8DA2-59949F14D6B3}"/>
+    <hyperlink ref="H65" r:id="rId153" xr:uid="{E01483F8-09F3-4452-BF30-1843E2DAC026}"/>
+    <hyperlink ref="H66" r:id="rId154" xr:uid="{420AE97C-C75D-4654-A5BC-2C6CD52393BE}"/>
+    <hyperlink ref="I63" r:id="rId155" xr:uid="{70DBAC93-6CC4-4257-B3CA-B596B587411B}"/>
+    <hyperlink ref="G5" r:id="rId156" xr:uid="{8D8D7438-B877-4D4B-9079-5A2E8D935A49}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>